<commit_message>
debug-Funktion für serial eingebaut
</commit_message>
<xml_diff>
--- a/docs/25pol Sub-D Belegung.xlsx
+++ b/docs/25pol Sub-D Belegung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c378eabe2b9b4f78/12 X-Plane/Teensy/MOSAM/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c378eabe2b9b4f78/12 X-Plane/Teensy/MOSAM/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51EAFE76-556F-4E62-8F31-D177D1543D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{51EAFE76-556F-4E62-8F31-D177D1543D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9C58060-CDC4-6B48-A65D-AB067815E98C}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2120" windowWidth="28800" windowHeight="15370" xr2:uid="{96D6205A-40B6-4C83-AEEE-26A4D07F9880}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20480" xr2:uid="{96D6205A-40B6-4C83-AEEE-26A4D07F9880}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -236,12 +236,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -271,12 +277,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -615,19 +624,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B2104E-7003-4FAE-A0AD-6B5DE3C8C7D5}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -655,7 +664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -669,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -681,7 +690,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -695,7 +704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -707,7 +716,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -719,7 +728,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -731,7 +740,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -743,7 +752,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -755,7 +764,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -767,7 +776,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -781,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -795,7 +804,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -807,8 +816,8 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
+    <row r="15" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2">
@@ -819,7 +828,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -831,7 +840,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -845,7 +854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -857,7 +866,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -869,7 +878,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -881,7 +890,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -893,7 +902,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -905,7 +914,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -917,7 +926,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -929,7 +938,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -943,7 +952,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>

</xml_diff>